<commit_message>
new notebook with new datta
</commit_message>
<xml_diff>
--- a/facebook_set/ranana.xlsx
+++ b/facebook_set/ranana.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19226"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20228"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\בתחן\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\erlichsefi\Google Drive\Running projects\מחקר ספורט\Code\facebook_set\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{EECFE862-8D67-4F45-A194-BA162D01D35D}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B01929D0-3463-4508-A3CC-31181D61BCDB}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7515" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -378,12 +378,12 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="177"/>
       <scheme val="minor"/>
@@ -391,14 +391,14 @@
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -509,8 +509,36 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD7D7D7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
+  <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2" xr9:uid="{570A79F4-53A2-40BE-A6F5-77C8D005F1F2}">
+      <tableStyleElement type="wholeTable" dxfId="1"/>
+      <tableStyleElement type="headerRow" dxfId="0"/>
+    </tableStyle>
+  </tableStyles>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -523,7 +551,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="ערכת נושא Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -825,91 +853,91 @@
       <selection activeCell="M26" sqref="M26:T26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
   <cols>
-    <col min="1" max="1" width="11.75" customWidth="1"/>
-    <col min="2" max="2" width="13.625" customWidth="1"/>
+    <col min="1" max="1" width="11.7265625" customWidth="1"/>
+    <col min="2" max="2" width="13.6328125" customWidth="1"/>
     <col min="3" max="3" width="17.5" customWidth="1"/>
-    <col min="5" max="5" width="22.375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="22.36328125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="25" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="26.125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="30.625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="31.625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="22.125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="28.125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="23.75" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="26.1328125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="30.6328125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="31.6328125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="22.1328125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="28.1328125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="23.7265625" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="26.5" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="27.75" customWidth="1"/>
+    <col min="15" max="15" width="27.7265625" customWidth="1"/>
     <col min="16" max="16" width="27.5" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="22.25" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="28.875" customWidth="1"/>
-    <col min="19" max="20" width="29.625" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="29.875" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="35.75" bestFit="1" customWidth="1"/>
-    <col min="23" max="24" width="30.125" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="25.625" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="31.125" bestFit="1" customWidth="1"/>
-    <col min="27" max="28" width="27.625" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="23.25" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="24.25" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="26.875" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="27.375" customWidth="1"/>
-    <col min="33" max="33" width="26.875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="22.2265625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="28.86328125" customWidth="1"/>
+    <col min="19" max="20" width="29.6328125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="29.86328125" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="35.7265625" bestFit="1" customWidth="1"/>
+    <col min="23" max="24" width="30.1328125" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="25.6328125" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="31.1328125" bestFit="1" customWidth="1"/>
+    <col min="27" max="28" width="27.6328125" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="23.2265625" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="24.2265625" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="26.86328125" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="27.36328125" customWidth="1"/>
+    <col min="33" max="33" width="26.86328125" bestFit="1" customWidth="1"/>
     <col min="34" max="34" width="30.5" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="24.25" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="22.125" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="27.375" customWidth="1"/>
-    <col min="38" max="38" width="26.875" customWidth="1"/>
-    <col min="39" max="39" width="30.875" customWidth="1"/>
-    <col min="40" max="40" width="31.375" customWidth="1"/>
-    <col min="41" max="41" width="30.75" customWidth="1"/>
-    <col min="42" max="42" width="24.25" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="24.2265625" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="22.1328125" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="27.36328125" customWidth="1"/>
+    <col min="38" max="38" width="26.86328125" customWidth="1"/>
+    <col min="39" max="39" width="30.86328125" customWidth="1"/>
+    <col min="40" max="40" width="31.36328125" customWidth="1"/>
+    <col min="41" max="41" width="30.7265625" customWidth="1"/>
+    <col min="42" max="42" width="24.2265625" bestFit="1" customWidth="1"/>
     <col min="43" max="43" width="26" customWidth="1"/>
-    <col min="44" max="44" width="36.375" bestFit="1" customWidth="1"/>
-    <col min="45" max="45" width="41.125" customWidth="1"/>
-    <col min="46" max="46" width="39.375" customWidth="1"/>
+    <col min="44" max="44" width="36.36328125" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="41.1328125" customWidth="1"/>
+    <col min="46" max="46" width="39.36328125" customWidth="1"/>
     <col min="47" max="47" width="30" bestFit="1" customWidth="1"/>
-    <col min="48" max="49" width="26.75" bestFit="1" customWidth="1"/>
-    <col min="50" max="50" width="27.375" customWidth="1"/>
-    <col min="51" max="52" width="28.75" bestFit="1" customWidth="1"/>
+    <col min="48" max="49" width="26.7265625" bestFit="1" customWidth="1"/>
+    <col min="50" max="50" width="27.36328125" customWidth="1"/>
+    <col min="51" max="52" width="28.7265625" bestFit="1" customWidth="1"/>
     <col min="53" max="53" width="33" bestFit="1" customWidth="1"/>
-    <col min="54" max="54" width="28.125" bestFit="1" customWidth="1"/>
+    <col min="54" max="54" width="28.1328125" bestFit="1" customWidth="1"/>
     <col min="55" max="55" width="31" bestFit="1" customWidth="1"/>
-    <col min="56" max="56" width="36.75" bestFit="1" customWidth="1"/>
-    <col min="57" max="57" width="37.25" bestFit="1" customWidth="1"/>
-    <col min="58" max="58" width="37.875" bestFit="1" customWidth="1"/>
-    <col min="59" max="59" width="38.875" customWidth="1"/>
-    <col min="60" max="60" width="38.875" bestFit="1" customWidth="1"/>
-    <col min="61" max="61" width="38.75" bestFit="1" customWidth="1"/>
-    <col min="62" max="62" width="41.375" bestFit="1" customWidth="1"/>
+    <col min="56" max="56" width="36.7265625" bestFit="1" customWidth="1"/>
+    <col min="57" max="57" width="37.2265625" bestFit="1" customWidth="1"/>
+    <col min="58" max="58" width="37.86328125" bestFit="1" customWidth="1"/>
+    <col min="59" max="59" width="38.86328125" customWidth="1"/>
+    <col min="60" max="60" width="38.86328125" bestFit="1" customWidth="1"/>
+    <col min="61" max="61" width="38.7265625" bestFit="1" customWidth="1"/>
+    <col min="62" max="62" width="41.36328125" bestFit="1" customWidth="1"/>
     <col min="63" max="65" width="42.5" bestFit="1" customWidth="1"/>
     <col min="66" max="66" width="43.5" bestFit="1" customWidth="1"/>
     <col min="67" max="68" width="44.5" bestFit="1" customWidth="1"/>
-    <col min="69" max="69" width="0.125" customWidth="1"/>
+    <col min="69" max="69" width="0.1328125" customWidth="1"/>
     <col min="70" max="70" width="36.5" bestFit="1" customWidth="1"/>
-    <col min="71" max="71" width="39.25" bestFit="1" customWidth="1"/>
-    <col min="72" max="74" width="40.25" bestFit="1" customWidth="1"/>
-    <col min="75" max="75" width="41.25" bestFit="1" customWidth="1"/>
-    <col min="76" max="76" width="42.875" bestFit="1" customWidth="1"/>
-    <col min="77" max="77" width="42.375" bestFit="1" customWidth="1"/>
-    <col min="78" max="78" width="42.25" bestFit="1" customWidth="1"/>
-    <col min="79" max="79" width="44.375" bestFit="1" customWidth="1"/>
+    <col min="71" max="71" width="39.2265625" bestFit="1" customWidth="1"/>
+    <col min="72" max="74" width="40.2265625" bestFit="1" customWidth="1"/>
+    <col min="75" max="75" width="41.2265625" bestFit="1" customWidth="1"/>
+    <col min="76" max="76" width="42.86328125" bestFit="1" customWidth="1"/>
+    <col min="77" max="77" width="42.36328125" bestFit="1" customWidth="1"/>
+    <col min="78" max="78" width="42.2265625" bestFit="1" customWidth="1"/>
+    <col min="79" max="79" width="44.36328125" bestFit="1" customWidth="1"/>
     <col min="80" max="82" width="46" bestFit="1" customWidth="1"/>
     <col min="83" max="83" width="47" bestFit="1" customWidth="1"/>
     <col min="84" max="85" width="48" bestFit="1" customWidth="1"/>
-    <col min="86" max="86" width="41.375" bestFit="1" customWidth="1"/>
-    <col min="87" max="87" width="44.125" bestFit="1" customWidth="1"/>
-    <col min="88" max="90" width="45.125" bestFit="1" customWidth="1"/>
-    <col min="91" max="91" width="46.25" bestFit="1" customWidth="1"/>
-    <col min="92" max="93" width="47.25" bestFit="1" customWidth="1"/>
-    <col min="94" max="94" width="47.125" bestFit="1" customWidth="1"/>
-    <col min="95" max="95" width="49.75" bestFit="1" customWidth="1"/>
-    <col min="96" max="98" width="50.875" bestFit="1" customWidth="1"/>
-    <col min="99" max="99" width="51.875" bestFit="1" customWidth="1"/>
-    <col min="100" max="101" width="52.875" bestFit="1" customWidth="1"/>
+    <col min="86" max="86" width="41.36328125" bestFit="1" customWidth="1"/>
+    <col min="87" max="87" width="44.1328125" bestFit="1" customWidth="1"/>
+    <col min="88" max="90" width="45.1328125" bestFit="1" customWidth="1"/>
+    <col min="91" max="91" width="46.2265625" bestFit="1" customWidth="1"/>
+    <col min="92" max="93" width="47.2265625" bestFit="1" customWidth="1"/>
+    <col min="94" max="94" width="47.1328125" bestFit="1" customWidth="1"/>
+    <col min="95" max="95" width="49.7265625" bestFit="1" customWidth="1"/>
+    <col min="96" max="98" width="50.86328125" bestFit="1" customWidth="1"/>
+    <col min="99" max="99" width="51.86328125" bestFit="1" customWidth="1"/>
+    <col min="100" max="101" width="52.86328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:101" ht="29.25" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:101" ht="45" thickBot="1" x14ac:dyDescent="0.9">
       <c r="A1" s="2" t="s">
         <v>5</v>
       </c>
@@ -1211,7 +1239,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="2" spans="1:101" ht="18.75" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:101" ht="18.25" x14ac:dyDescent="0.75">
       <c r="A2" s="13">
         <v>42966</v>
       </c>
@@ -1513,7 +1541,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:101" ht="18.75" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:101" ht="18.25" x14ac:dyDescent="0.75">
       <c r="A3" s="13">
         <v>42973</v>
       </c>
@@ -1815,7 +1843,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:101" ht="18.75" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:101" ht="18.25" x14ac:dyDescent="0.75">
       <c r="A4" s="13">
         <v>42988</v>
       </c>
@@ -2117,7 +2145,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:101" ht="18.75" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:101" ht="18.25" x14ac:dyDescent="0.75">
       <c r="A5" s="13">
         <v>42994</v>
       </c>
@@ -2419,7 +2447,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:101" ht="18.75" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:101" ht="18.25" x14ac:dyDescent="0.75">
       <c r="A6" s="13">
         <v>43001</v>
       </c>
@@ -2721,7 +2749,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:101" ht="18.75" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:101" ht="18.25" x14ac:dyDescent="0.75">
       <c r="A7" s="13">
         <v>43009</v>
       </c>
@@ -3023,7 +3051,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:101" ht="18.75" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:101" ht="18.25" x14ac:dyDescent="0.75">
       <c r="A8" s="13">
         <v>43022</v>
       </c>
@@ -3325,7 +3353,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:101" ht="18.75" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:101" ht="18.25" x14ac:dyDescent="0.75">
       <c r="A9" s="13">
         <v>43029</v>
       </c>
@@ -3627,7 +3655,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:101" ht="18.75" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:101" ht="18.25" x14ac:dyDescent="0.75">
       <c r="A10" s="13">
         <v>43036</v>
       </c>
@@ -3929,7 +3957,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:101" ht="18.75" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:101" ht="18.25" x14ac:dyDescent="0.75">
       <c r="A11" s="13">
         <v>43044</v>
       </c>
@@ -4231,7 +4259,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:101" ht="18.75" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:101" ht="18.25" x14ac:dyDescent="0.75">
       <c r="A12" s="13">
         <v>43065</v>
       </c>
@@ -4533,7 +4561,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:101" ht="18.75" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:101" ht="18.25" x14ac:dyDescent="0.75">
       <c r="A13" s="13">
         <v>43072</v>
       </c>
@@ -4835,7 +4863,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:101" ht="18.75" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:101" ht="18.25" x14ac:dyDescent="0.75">
       <c r="A14" s="13">
         <v>43078</v>
       </c>
@@ -5137,7 +5165,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:101" ht="18.75" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:101" ht="18.25" x14ac:dyDescent="0.75">
       <c r="A15" s="13">
         <v>43086</v>
       </c>
@@ -5439,7 +5467,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:101" ht="18.75" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:101" ht="18.25" x14ac:dyDescent="0.75">
       <c r="A16" s="13">
         <v>43093</v>
       </c>
@@ -5741,7 +5769,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:106" ht="18.75" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:106" ht="18.25" x14ac:dyDescent="0.75">
       <c r="A17" s="13">
         <v>43099</v>
       </c>
@@ -6043,7 +6071,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:106" ht="18.75" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:106" ht="18.25" x14ac:dyDescent="0.75">
       <c r="A18" s="13">
         <v>43110</v>
       </c>
@@ -6345,7 +6373,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:106" ht="18.75" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:106" ht="18.25" x14ac:dyDescent="0.75">
       <c r="A19" s="13">
         <v>43114</v>
       </c>
@@ -6647,7 +6675,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:106" ht="18.75" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:106" ht="18.25" x14ac:dyDescent="0.75">
       <c r="A20" s="13">
         <v>43120</v>
       </c>
@@ -6954,7 +6982,7 @@
       <c r="DA20" s="14"/>
       <c r="DB20" s="14"/>
     </row>
-    <row r="21" spans="1:106" ht="18.75" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:106" ht="18.25" x14ac:dyDescent="0.75">
       <c r="A21" s="13">
         <v>43127</v>
       </c>
@@ -7256,7 +7284,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:106" ht="18.75" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:106" ht="18.25" x14ac:dyDescent="0.75">
       <c r="A22" s="13">
         <v>43134</v>
       </c>
@@ -7558,7 +7586,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:106" ht="18.75" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:106" ht="18.25" x14ac:dyDescent="0.75">
       <c r="A23" s="13">
         <v>43141</v>
       </c>
@@ -7860,7 +7888,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:106" ht="18.75" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:106" ht="18.25" x14ac:dyDescent="0.75">
       <c r="A24" s="13">
         <v>43148</v>
       </c>
@@ -8162,7 +8190,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:106" ht="18.75" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:106" ht="18.25" x14ac:dyDescent="0.75">
       <c r="A25" s="13">
         <v>43155</v>
       </c>
@@ -8464,7 +8492,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:106" ht="18.75" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:106" ht="18.25" x14ac:dyDescent="0.75">
       <c r="A26" s="13">
         <v>43162</v>
       </c>
@@ -8766,7 +8794,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:106" ht="18.75" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:106" ht="18.25" x14ac:dyDescent="0.75">
       <c r="A27" s="13">
         <v>43160</v>
       </c>
@@ -9068,7 +9096,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:106" ht="18.75" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:106" ht="18.25" x14ac:dyDescent="0.75">
       <c r="A28" s="13">
         <v>43177</v>
       </c>
@@ -9370,7 +9398,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:106" ht="18.75" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:106" ht="18.25" x14ac:dyDescent="0.75">
       <c r="A29" s="13">
         <v>43197</v>
       </c>
@@ -9672,7 +9700,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:106" ht="18.75" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:106" ht="18.25" x14ac:dyDescent="0.75">
       <c r="A30" s="13">
         <v>43204</v>
       </c>
@@ -9974,7 +10002,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:106" ht="18.75" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:106" ht="18.25" x14ac:dyDescent="0.75">
       <c r="A31" s="13">
         <v>43213</v>
       </c>
@@ -10276,7 +10304,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:106" ht="18.75" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:106" ht="18.25" x14ac:dyDescent="0.75">
       <c r="A32" s="13">
         <v>43218</v>
       </c>
@@ -10578,7 +10606,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:101" ht="18.75" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:101" ht="18.25" x14ac:dyDescent="0.75">
       <c r="A33" s="13">
         <v>43226</v>
       </c>
@@ -10880,7 +10908,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:101" ht="18.75" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:101" ht="18.25" x14ac:dyDescent="0.75">
       <c r="A34" s="13">
         <v>43233</v>
       </c>
@@ -11182,7 +11210,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:101" ht="18.75" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:101" ht="18.25" x14ac:dyDescent="0.75">
       <c r="D35" s="1"/>
       <c r="BA35" s="14"/>
       <c r="BB35" s="14"/>
@@ -11193,19 +11221,19 @@
       <c r="BG35" s="14"/>
       <c r="BH35" s="14"/>
     </row>
-    <row r="36" spans="1:101" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:101" x14ac:dyDescent="0.75">
       <c r="D36" s="1"/>
     </row>
-    <row r="37" spans="1:101" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:101" x14ac:dyDescent="0.75">
       <c r="D37" s="1"/>
     </row>
-    <row r="38" spans="1:101" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:101" x14ac:dyDescent="0.75">
       <c r="D38" s="1"/>
     </row>
-    <row r="39" spans="1:101" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:101" x14ac:dyDescent="0.75">
       <c r="D39" s="1"/>
     </row>
-    <row r="40" spans="1:101" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:101" x14ac:dyDescent="0.75">
       <c r="D40" s="1"/>
     </row>
   </sheetData>

</xml_diff>